<commit_message>
Datos & Shapiro-Wilk Test
</commit_message>
<xml_diff>
--- a/Proyecto Final/Info/Info.xlsx
+++ b/Proyecto Final/Info/Info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DERS\Documents\GitHub\ESTADISTICA-PROYECTO\Proyecto Final\Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathy\Documents\GitHub\ESTADISTICA-PROYECTO\Proyecto Final\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C22CF22-BBA0-4BEF-B81F-5E3A172F24E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183B3E47-D35A-4370-BCA7-9CFC20D0CD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="23">
   <si>
     <t>Edad</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Algo fácil</t>
-  </si>
-  <si>
-    <t>Excelente</t>
   </si>
   <si>
     <t>Laboral</t>
@@ -524,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,37 +535,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
       <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
         <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -664,7 +661,7 @@
         <v>90</v>
       </c>
       <c r="F4" s="1">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G4" s="1">
         <v>1000</v>
@@ -786,7 +783,7 @@
       <c r="H7" s="1">
         <v>600</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>9</v>
       </c>
       <c r="J7" s="1">
@@ -865,8 +862,8 @@
       <c r="I9" s="1">
         <v>11</v>
       </c>
-      <c r="J9" s="1">
-        <v>9</v>
+      <c r="J9" s="2">
+        <v>8.4</v>
       </c>
       <c r="K9" s="1">
         <v>4</v>
@@ -1169,8 +1166,8 @@
       <c r="I17" s="1">
         <v>16</v>
       </c>
-      <c r="J17" s="1">
-        <v>6</v>
+      <c r="J17" s="2">
+        <v>6.4</v>
       </c>
       <c r="K17" s="1">
         <v>5</v>
@@ -1268,8 +1265,8 @@
       <c r="D20" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="1">
-        <v>20</v>
+      <c r="E20" s="2">
+        <v>40</v>
       </c>
       <c r="F20" s="1">
         <v>15</v>
@@ -1538,7 +1535,7 @@
         <v>25</v>
       </c>
       <c r="F27" s="1">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G27" s="1">
         <v>400</v>
@@ -1646,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E30" s="1">
         <v>35</v>
@@ -2005,8 +2002,8 @@
       <c r="I39" s="1">
         <v>9</v>
       </c>
-      <c r="J39" s="1">
-        <v>6</v>
+      <c r="J39" s="2">
+        <v>6.45</v>
       </c>
       <c r="K39" s="1">
         <v>4</v>
@@ -2294,11 +2291,11 @@
       <c r="D47" t="s">
         <v>3</v>
       </c>
-      <c r="E47" s="1">
-        <v>60</v>
+      <c r="E47" s="2">
+        <v>45</v>
       </c>
       <c r="F47" s="1">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G47" s="1">
         <v>150</v>
@@ -2309,8 +2306,8 @@
       <c r="I47" s="1">
         <v>12</v>
       </c>
-      <c r="J47" s="1">
-        <v>9</v>
+      <c r="J47" s="2">
+        <v>8.8000000000000007</v>
       </c>
       <c r="K47" s="1">
         <v>8</v>
@@ -2450,7 +2447,7 @@
         <v>85</v>
       </c>
       <c r="F51" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G51" s="1">
         <v>2500</v>

</xml_diff>